<commit_message>
Updates to test framework
</commit_message>
<xml_diff>
--- a/Test_Framework/_Tests.xlsx
+++ b/Test_Framework/_Tests.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EF8AFD-7F60-4061-B494-091733D5183E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="1524" windowWidth="22344" windowHeight="7332" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="13">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -56,12 +57,18 @@
   </si>
   <si>
     <t>Framework\InitAllApplications.xaml</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>No exception thrown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,7 +397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -564,7 +571,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>
@@ -574,7 +581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -644,7 +651,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -768,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -779,7 +789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -790,7 +800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -798,10 +808,13 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -809,13 +822,16 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>